<commit_message>
load balancer is completd
</commit_message>
<xml_diff>
--- a/cem-eng-cxo_nagios_review.xlsx
+++ b/cem-eng-cxo_nagios_review.xlsx
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="281">
   <si>
     <t>S no</t>
   </si>
@@ -1008,6 +1008,9 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -1550,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1570,7 +1573,7 @@
     <col min="10" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -1597,7 +1600,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="32">
         <v>1</v>
       </c>
@@ -1623,8 +1626,11 @@
       <c r="I2" s="32" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J2" s="31" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="32">
         <v>2</v>
       </c>
@@ -1651,7 +1657,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="32">
         <v>3</v>
       </c>
@@ -1678,7 +1684,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="32">
         <v>4</v>
       </c>
@@ -1705,7 +1711,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="32">
         <v>5</v>
       </c>
@@ -1732,7 +1738,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="32">
         <v>6</v>
       </c>
@@ -1757,7 +1763,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="32">
         <v>7</v>
       </c>
@@ -1782,7 +1788,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="32">
         <v>8</v>
       </c>
@@ -1803,7 +1809,7 @@
       <c r="H9" s="32"/>
       <c r="I9" s="32"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="32">
         <v>9</v>
       </c>
@@ -1828,7 +1834,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="32">
         <v>10</v>
       </c>
@@ -1853,7 +1859,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="32">
         <v>11</v>
       </c>
@@ -1880,7 +1886,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="32"/>
       <c r="B13" s="33"/>
       <c r="C13" s="33"/>
@@ -1891,7 +1897,7 @@
       <c r="H13" s="32"/>
       <c r="I13" s="32"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="32">
         <v>12</v>
       </c>
@@ -1908,7 +1914,7 @@
       <c r="H14" s="32"/>
       <c r="I14" s="32"/>
     </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="32">
         <v>13</v>
       </c>
@@ -1927,7 +1933,7 @@
       <c r="H15" s="32"/>
       <c r="I15" s="32"/>
     </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="32">
         <v>14</v>
       </c>

</xml_diff>